<commit_message>
New Demo Import App + sample files
</commit_message>
<xml_diff>
--- a/com.servicenow.processmining.extensions/applications/demodata/samples/Incident Demo Data.xlsx
+++ b/com.servicenow.processmining.extensions/applications/demodata/samples/Incident Demo Data.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eduardo.chiocconi/Desktop/Demo Scripts/Incidents Evaluation Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eduardo.chiocconi/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{969C04A6-EE58-0D47-9603-83953DB1D755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A6D05B-4B3A-B842-A102-9B90A55C0A24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33000" yWindow="3480" windowWidth="28040" windowHeight="17440" xr2:uid="{DC4B5DAD-EB22-8246-A4DA-9BF66107CB35}"/>
+    <workbookView xWindow="34820" yWindow="1600" windowWidth="28040" windowHeight="17440" activeTab="5" xr2:uid="{DC4B5DAD-EB22-8246-A4DA-9BF66107CB35}"/>
   </bookViews>
   <sheets>
     <sheet name="Path-1" sheetId="1" r:id="rId1"/>
+    <sheet name="Path-1-1" sheetId="6" r:id="rId2"/>
+    <sheet name="Path-2-1" sheetId="2" r:id="rId3"/>
+    <sheet name="Path-2-2" sheetId="4" r:id="rId4"/>
+    <sheet name="Path-3-1" sheetId="3" r:id="rId5"/>
+    <sheet name="Path-3-2" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="181029" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="42">
   <si>
     <t>Table</t>
   </si>
@@ -86,9 +91,6 @@
     <t>Intermitent network issues, Out of network, Network outage, Wifi problems, VPN network issues</t>
   </si>
   <si>
-    <t>PM: Path-1</t>
-  </si>
-  <si>
     <t>assignment_group</t>
   </si>
   <si>
@@ -141,13 +143,37 @@
   </si>
   <si>
     <t>close_notes</t>
+  </si>
+  <si>
+    <t>Wifi still not working.</t>
+  </si>
+  <si>
+    <t>Slow transition</t>
+  </si>
+  <si>
+    <t>Helpdesk L2</t>
+  </si>
+  <si>
+    <t>Helpdesk L3</t>
+  </si>
+  <si>
+    <t>Assigned to Helpdesk L1 group.</t>
+  </si>
+  <si>
+    <t>Assigned to Helpdesk L1  group.</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>PMAgentic2: Path-1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -160,6 +186,19 @@
       <color rgb="FFCCCCCC"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -182,12 +221,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB58E369-E6B1-5C40-B243-82E8DEF89FA7}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,49 +589,45 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2">
-        <v>60</v>
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="6">
+        <v>44927</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>600</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -594,13 +635,10 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -608,10 +646,13 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -619,10 +660,10 @@
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -630,10 +671,10 @@
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -641,21 +682,21 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>3600</v>
+        <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -663,10 +704,10 @@
         <v>3600</v>
       </c>
       <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -674,10 +715,10 @@
         <v>3600</v>
       </c>
       <c r="B14" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -685,21 +726,21 @@
         <v>3600</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>9000</v>
+        <v>3600</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -707,71 +748,1665 @@
         <v>9000</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>12000</v>
+        <v>9000</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>12000</v>
+        <v>14000</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="2"/>
+        <v>23</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>12000</v>
+        <v>14000</v>
       </c>
       <c r="B20" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>12000</v>
+        <v>14000</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>15000</v>
+        <v>14000</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
+      </c>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>16000</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA91FB9-5BA3-7A40-9E8E-0D612BB0A2E5}">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="6">
+        <v>44927</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>3600</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>3600</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>3600</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>3600</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>9000</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>9000</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>10000</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>10000</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>10000</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>10000</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>11000</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC6710E0-97DF-A64C-85A9-D89665087DAF}">
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="6">
+        <v>45292</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3">
+        <v>600</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>0</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>0</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>0</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>0</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>0</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>3600</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>3600</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>3600</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>3600</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>9000</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>9000</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>12000</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>12000</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>12000</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>12000</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>15000</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>15000</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>20000</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>20000</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>20000</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>20000</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>23000</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="3">
+        <v>23000</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <v>30000</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>30000</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="3">
+        <v>30000</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="3">
+        <v>30000</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="3">
+        <v>32000</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4AFEE56-A323-1749-BEBD-ABF7CD027EED}">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="6">
+        <v>45292</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3">
+        <v>600</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>0</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>0</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>0</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>0</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>0</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>0</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>3600</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>3600</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>3600</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>3600</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>9000</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>9000</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>12000</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>12000</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="3">
+        <v>12000</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="3">
+        <v>12000</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="3">
+        <v>15000</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>15000</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="3">
+        <v>20000</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="3">
+        <v>20000</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="3">
+        <v>20000</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="3">
+        <v>20000</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="3">
+        <v>22000</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56CE2401-A9FF-AA44-85B9-1AC3FCF991D1}">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="6">
+        <v>45658</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3">
+        <v>600</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>3600</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>3600</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>3600</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>3600</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>4600</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>4600</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>10000</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>10000</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>13000</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>13000</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>13000</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>13000</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>15000</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F64903-5C9B-A64A-A1DE-88BE389F76AA}">
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="6">
+        <v>45658</v>
+      </c>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3">
+        <v>600</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>3600</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>3600</v>
+      </c>
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>3600</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>3600</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>4600</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>6600</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>12000</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>12000</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>15000</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>15000</v>
+      </c>
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>15000</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>15000</v>
+      </c>
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>17000</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="4"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="4"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="4"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="4"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="4"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{8bcff170-9979-491e-8683-d8ced0850bad}" enabled="0" method="" siteId="{8bcff170-9979-491e-8683-d8ced0850bad}" removed="1"/>
+</clbl:labelList>
 </file>
</xml_diff>